<commit_message>
plots e recopy of datasets
</commit_message>
<xml_diff>
--- a/Ammonium.xlsx
+++ b/Ammonium.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\UDESC\ThermoPhase - 2024\Testes de Consistência\consistency_tests_2024-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C1D57D-1CEA-47D5-ABE8-52E5EA8EE041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57A1361-8948-4E15-9080-0DA624661873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{AD13E020-50D9-4923-829C-632D7D081214}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="10245" windowHeight="8715" firstSheet="28" activeTab="28" xr2:uid="{AD13E020-50D9-4923-829C-632D7D081214}"/>
   </bookViews>
   <sheets>
     <sheet name="deahso4_1_gupta" sheetId="1" r:id="rId1"/>
@@ -341,7 +341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -393,6 +393,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -404,7 +405,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,13 +723,15 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -794,10 +797,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1">
@@ -871,8 +874,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C5" si="0">D3-273.15</f>
         <v>9.0400000000000205</v>
@@ -894,7 +897,7 @@
       <c r="H3" s="11">
         <v>282.61582977425536</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="27">
         <f t="shared" ref="I3:I5" si="3">F3-10^(-4646.471 +5314653/H3 -2271392000/H3^2 +430306500000/H3^3 -30511740000000/H3^4)</f>
         <v>-2.0541790490824496E-11</v>
       </c>
@@ -920,8 +923,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>7.5400000000000205</v>
@@ -969,8 +972,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>4.4399999999999977</v>
@@ -1031,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08785D87-6D68-4A89-9CC4-11C359CF470C}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,10 +1107,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1">
@@ -1178,8 +1181,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.0500000000000007</v>
       </c>
@@ -1224,8 +1227,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>12.19</v>
       </c>
@@ -1270,8 +1273,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>13.25</v>
       </c>
@@ -1328,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBD1D50-D3CF-429E-89E4-D678955B9271}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,10 +1404,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="7">
@@ -1478,8 +1481,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C6" si="7">D3-273.15</f>
         <v>5.4500000000000455</v>
@@ -1527,8 +1530,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="7"/>
         <v>9.0500000000000114</v>
@@ -1576,8 +1579,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="7"/>
         <v>10.050000000000011</v>
@@ -1625,8 +1628,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7">
         <f t="shared" si="7"/>
         <v>11.100000000000023</v>
@@ -1686,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA0FC79-3596-432A-A080-AA1677D15641}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,10 +1762,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="7">
@@ -1836,8 +1839,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
         <v>5.25</v>
@@ -1885,8 +1888,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>8.8500000000000227</v>
@@ -1934,8 +1937,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>9.8500000000000227</v>
@@ -1983,8 +1986,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>10.950000000000045</v>
@@ -2044,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB3747F-CF12-46F7-A892-B1E5A8E36E67}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,10 +2119,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="7">
@@ -2191,8 +2194,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C6" si="8">D3-273.15</f>
         <v>4.8500000000000227</v>
@@ -2238,8 +2241,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="8"/>
         <v>8.3500000000000227</v>
@@ -2285,8 +2288,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="8"/>
         <v>9.3500000000000227</v>
@@ -2332,8 +2335,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7">
         <f t="shared" si="8"/>
         <v>10.350000000000023</v>
@@ -2392,8 +2395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0FA3371-2A2E-491D-95E1-4FEEFE4E9536}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,10 +2468,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="7">
@@ -2542,8 +2545,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
         <v>5.5500000000000114</v>
@@ -2591,8 +2594,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>9.1500000000000341</v>
@@ -2640,8 +2643,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>10.100000000000023</v>
@@ -2689,8 +2692,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>11.150000000000034</v>
@@ -2750,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2B8822-8897-4A20-955E-AC23CCF77FE9}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,10 +2826,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>38</v>
       </c>
       <c r="C2" s="7">
@@ -2900,8 +2903,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" si="0"/>
         <v>5.3500000000000227</v>
@@ -2949,8 +2952,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="0"/>
         <v>8.9500000000000455</v>
@@ -2998,8 +3001,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="0"/>
         <v>9.9700000000000273</v>
@@ -3047,8 +3050,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
         <v>10.950000000000045</v>
@@ -3108,8 +3111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA50A75-4EB2-4C93-84C2-370EF568DC6A}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,10 +3184,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
       <c r="C2" s="7">
@@ -3256,8 +3259,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="7">
         <f t="shared" ref="C3:C5" si="9">D3-273.15</f>
         <v>9.4800000000000182</v>
@@ -3303,8 +3306,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="7">
         <f t="shared" si="9"/>
         <v>12.29000000000002</v>
@@ -3350,8 +3353,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="7">
         <f t="shared" si="9"/>
         <v>13.470000000000027</v>
@@ -3409,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67611EF-28CB-40F9-AB0D-8FAD486E785E}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:U1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,10 +3485,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="1">
@@ -3556,8 +3559,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>4.95</v>
       </c>
@@ -3602,8 +3605,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>8.5500000000000007</v>
       </c>
@@ -3648,8 +3651,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>9.5500000000000007</v>
       </c>
@@ -3694,8 +3697,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>10.65</v>
       </c>
@@ -3752,8 +3755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555CE77F-4728-4976-97B7-4196E905D026}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3825,10 +3828,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C2" s="1">
@@ -3899,8 +3902,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>9.56</v>
       </c>
@@ -3945,8 +3948,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>11.17</v>
       </c>
@@ -3991,8 +3994,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>13.29</v>
       </c>
@@ -4037,8 +4040,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>14.6</v>
       </c>
@@ -4095,8 +4098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA6F2D3-40E1-4EA3-8AC0-4E17C598B937}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4168,10 +4171,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>44</v>
       </c>
       <c r="C2" s="1">
@@ -4242,8 +4245,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>7.72</v>
       </c>
@@ -4288,8 +4291,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>10.44</v>
       </c>
@@ -4334,8 +4337,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>11.84</v>
       </c>
@@ -4380,8 +4383,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>12.19</v>
       </c>
@@ -4438,14 +4441,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE3DAAD-7B8C-429B-990A-0D207C2176F5}">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -4511,10 +4515,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C2" s="9">
@@ -4585,8 +4589,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="9">
         <v>7.46</v>
       </c>
@@ -4631,8 +4635,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="24"/>
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="9">
         <v>9.9700000000000006</v>
       </c>
@@ -4677,8 +4681,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="9">
         <v>12.12</v>
       </c>
@@ -4738,7 +4742,7 @@
       <c r="Q6" s="4"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="M10" s="26"/>
+      <c r="M10" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4754,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0D31C94-6E49-4D6A-89AB-F48CD1CD2366}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4827,10 +4831,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>45</v>
       </c>
       <c r="C2" s="1">
@@ -4904,8 +4908,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C6" si="8">D3-273.15</f>
         <v>5.4000000000000341</v>
@@ -4953,8 +4957,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <f t="shared" si="8"/>
         <v>8.9000000000000341</v>
@@ -5002,8 +5006,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <f t="shared" si="8"/>
         <v>9.9500000000000455</v>
@@ -5051,8 +5055,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <f t="shared" si="8"/>
         <v>11</v>
@@ -5112,8 +5116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32988DA5-3E8A-453E-BF6A-E4AA4A2C8FA9}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5185,10 +5189,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="1">
@@ -5262,8 +5266,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
         <v>5.0500000000000114</v>
@@ -5311,8 +5315,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>8.4500000000000455</v>
@@ -5360,8 +5364,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>9.75</v>
@@ -5409,8 +5413,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>10.75</v>
@@ -5470,8 +5474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95F232B-C6E8-48D0-A24B-38DE49BC84C9}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T1" sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5543,10 +5547,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>47</v>
       </c>
       <c r="C2" s="1">
@@ -5617,8 +5621,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>4.55</v>
       </c>
@@ -5663,8 +5667,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>7.95</v>
       </c>
@@ -5709,8 +5713,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>9.15</v>
       </c>
@@ -5755,8 +5759,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>10.050000000000001</v>
       </c>
@@ -5813,8 +5817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{535BF539-98F4-4FDE-8CA2-58265B10109F}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,10 +5890,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="1">
@@ -5960,8 +5964,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.4499999999999993</v>
       </c>
@@ -6006,8 +6010,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>5.35</v>
       </c>
@@ -6052,8 +6056,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>2.75</v>
       </c>
@@ -6110,8 +6114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A502364A-3E0D-4EFE-84F4-601027FF1FAB}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6183,10 +6187,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="1">
@@ -6257,8 +6261,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.9499999999999993</v>
       </c>
@@ -6303,8 +6307,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>6.05</v>
       </c>
@@ -6349,8 +6353,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>3.45</v>
       </c>
@@ -6408,7 +6412,7 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:T1"/>
+      <selection sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6480,10 +6484,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="1">
@@ -6554,8 +6558,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.4499999999999993</v>
       </c>
@@ -6600,8 +6604,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>5.35</v>
       </c>
@@ -6646,8 +6650,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>2.75</v>
       </c>
@@ -6704,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{307813F3-D709-4DC6-8D97-D40DCC8A28CD}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6777,10 +6781,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="2">
@@ -6854,8 +6858,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2">
         <f t="shared" ref="C3:C5" si="7">D3-273.15</f>
         <v>5.5500000000000114</v>
@@ -6903,8 +6907,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2">
         <f t="shared" si="7"/>
         <v>8.75</v>
@@ -6952,8 +6956,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2">
         <f t="shared" si="7"/>
         <v>10.75</v>
@@ -7013,8 +7017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70B30C08-A0B6-4FE6-8F6A-787C42331F51}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7086,10 +7090,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>54</v>
       </c>
       <c r="C2" s="2">
@@ -7163,8 +7167,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2">
         <f t="shared" si="0"/>
         <v>5.4500000000000455</v>
@@ -7212,8 +7216,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>8.3500000000000227</v>
@@ -7261,8 +7265,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>10.550000000000011</v>
@@ -7322,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8531D5-7709-495E-80EA-50064B046BDF}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7395,10 +7399,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="2">
@@ -7472,8 +7476,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2">
         <f t="shared" si="0"/>
         <v>5.25</v>
@@ -7521,8 +7525,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="2">
         <f t="shared" si="0"/>
         <v>8.25</v>
@@ -7570,8 +7574,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>10.25</v>
@@ -7631,8 +7635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D89F90E-9983-4649-A575-C26B365ADD18}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7704,10 +7708,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="16">
@@ -7781,8 +7785,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="16">
         <f t="shared" ref="C3:C6" si="8">D3-273.15</f>
         <v>9.0361000000000331</v>
@@ -7830,8 +7834,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="16">
         <f t="shared" si="8"/>
         <v>7.7367000000000417</v>
@@ -7879,8 +7883,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="16">
         <f t="shared" si="8"/>
         <v>6.4372000000000185</v>
@@ -7928,8 +7932,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="16">
         <f t="shared" si="8"/>
         <v>3.5384000000000242</v>
@@ -7989,8 +7993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8CEFB8-82F5-4F15-A3D9-2E766A5AEA93}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8062,10 +8066,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="1">
@@ -8136,8 +8140,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>9.23</v>
       </c>
@@ -8182,8 +8186,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>11.04</v>
       </c>
@@ -8241,7 +8245,7 @@
   <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8313,10 +8317,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>58</v>
       </c>
       <c r="C2" s="16">
@@ -8390,8 +8394,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="16">
         <f t="shared" si="0"/>
         <v>8.5363000000000397</v>
@@ -8439,8 +8443,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="16">
         <f t="shared" si="0"/>
         <v>7.2369000000000483</v>
@@ -8488,8 +8492,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
       <c r="C5" s="16">
         <f t="shared" si="0"/>
         <v>5.6375000000000455</v>
@@ -8537,8 +8541,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
       <c r="C6" s="16">
         <f t="shared" si="0"/>
         <v>3.7383000000000379</v>
@@ -8598,8 +8602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD93ED6-BA62-4C76-9AA5-899D2F1047B0}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8671,10 +8675,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="1">
@@ -8745,8 +8749,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>7.26</v>
       </c>
@@ -8791,8 +8795,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>10.11</v>
       </c>
@@ -8837,8 +8841,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>11.82</v>
       </c>
@@ -8895,8 +8899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F059F784-65B3-46AC-BA41-48E42D81E9EF}">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8968,10 +8972,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C2" s="1">
@@ -9042,8 +9046,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.6199999999999992</v>
       </c>
@@ -9088,8 +9092,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>11.077999999999999</v>
       </c>
@@ -9146,8 +9150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69116A5-2E86-45B0-AECF-61B822B1E60E}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T1" sqref="A1:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9219,10 +9223,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>30</v>
       </c>
       <c r="C2" s="1">
@@ -9293,8 +9297,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>7.61</v>
       </c>
@@ -9339,8 +9343,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>10.15</v>
       </c>
@@ -9385,8 +9389,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>11.98</v>
       </c>
@@ -9444,7 +9448,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9516,10 +9520,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="1">
@@ -9590,8 +9594,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.44</v>
       </c>
@@ -9636,8 +9640,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>11.73</v>
       </c>
@@ -9694,8 +9698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1352D17-46DF-4CF6-8312-A32A284DAFD7}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection sqref="A1:T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9767,10 +9771,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C2" s="1">
@@ -9841,8 +9845,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>2.35</v>
       </c>
@@ -9887,8 +9891,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>4.3499999999999996</v>
       </c>
@@ -9933,8 +9937,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>5.45</v>
       </c>
@@ -9979,8 +9983,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>6.65</v>
       </c>
@@ -10025,8 +10029,8 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="1">
         <v>7.75</v>
       </c>
@@ -10071,8 +10075,8 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="1">
         <v>8.5500000000000007</v>
       </c>
@@ -10117,8 +10121,8 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="1">
         <v>9.5500000000000007</v>
       </c>
@@ -10163,8 +10167,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="1">
         <v>9.9499999999999993</v>
       </c>
@@ -10209,8 +10213,8 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="1">
         <v>10.25</v>
       </c>
@@ -10267,8 +10271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07C9F67-F356-47F0-838B-4288FAA31507}">
   <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:T1"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10340,10 +10344,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="1">
@@ -10414,8 +10418,8 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1">
         <v>8.3000000000000007</v>
       </c>
@@ -10460,8 +10464,8 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1">
         <v>10.51</v>
       </c>
@@ -10506,8 +10510,8 @@
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1">
         <v>12.32</v>
       </c>
@@ -10552,8 +10556,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1">
         <v>13.93</v>
       </c>

</xml_diff>